<commit_message>
clean common_parameters (not finished)
</commit_message>
<xml_diff>
--- a/spreadsheets/common_parameters.xlsx
+++ b/spreadsheets/common_parameters.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20343"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20344"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rrag0004\Models\SNAP_TB_BMC_MED\spreadsheets\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rrag0004\Models\SNAP-TB_new\spreadsheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{657583C5-C23F-4358-81C8-52E7A16538F7}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CDE70682-F8D3-42EC-9879-95E439DA40A1}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16400" windowHeight="6600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16395" windowHeight="6600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="constant" sheetId="1" r:id="rId1"/>
@@ -807,18 +807,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D80"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" zoomScale="205" zoomScaleNormal="205" workbookViewId="0">
-      <selection activeCell="B32" sqref="B32"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="205" zoomScaleNormal="205" workbookViewId="0">
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="37.7265625" customWidth="1"/>
-    <col min="2" max="2" width="11.7265625" customWidth="1"/>
-    <col min="4" max="4" width="65.7265625" customWidth="1"/>
+    <col min="1" max="1" width="37.7109375" customWidth="1"/>
+    <col min="2" max="2" width="11.7109375" customWidth="1"/>
+    <col min="4" max="4" width="65.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="10" t="s">
         <v>49</v>
       </c>
@@ -830,7 +830,7 @@
       </c>
       <c r="D1" s="10"/>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="10" t="s">
         <v>2</v>
       </c>
@@ -844,7 +844,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="11" t="s">
         <v>50</v>
       </c>
@@ -856,7 +856,7 @@
       </c>
       <c r="D3" s="11"/>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="11" t="s">
         <v>51</v>
       </c>
@@ -868,7 +868,7 @@
       </c>
       <c r="D4" s="11"/>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="11" t="s">
         <v>52</v>
       </c>
@@ -882,7 +882,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="11" t="s">
         <v>15</v>
       </c>
@@ -894,7 +894,7 @@
       </c>
       <c r="D6" s="11"/>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="11" t="s">
         <v>16</v>
       </c>
@@ -906,7 +906,7 @@
       </c>
       <c r="D7" s="11"/>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="11" t="s">
         <v>17</v>
       </c>
@@ -920,7 +920,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="11" t="s">
         <v>18</v>
       </c>
@@ -934,7 +934,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="11" t="s">
         <v>53</v>
       </c>
@@ -946,7 +946,7 @@
       </c>
       <c r="D10" s="11"/>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="9" t="s">
         <v>102</v>
       </c>
@@ -960,7 +960,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="9" t="s">
         <v>101</v>
       </c>
@@ -974,7 +974,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="9" t="s">
         <v>20</v>
       </c>
@@ -988,7 +988,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="9" t="s">
         <v>74</v>
       </c>
@@ -1002,7 +1002,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="9" t="s">
         <v>75</v>
       </c>
@@ -1016,7 +1016,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="16" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="14" t="s">
         <v>78</v>
       </c>
@@ -1030,7 +1030,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="17" spans="1:4" ht="15" thickTop="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:4" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A17" s="12" t="s">
         <v>14</v>
       </c>
@@ -1044,7 +1044,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="7" t="s">
         <v>113</v>
       </c>
@@ -1056,7 +1056,7 @@
       </c>
       <c r="D18" s="7"/>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="7" t="s">
         <v>114</v>
       </c>
@@ -1070,7 +1070,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="7" t="s">
         <v>115</v>
       </c>
@@ -1084,7 +1084,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="7" t="s">
         <v>11</v>
       </c>
@@ -1096,7 +1096,7 @@
       </c>
       <c r="D21" s="7"/>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="7" t="s">
         <v>13</v>
       </c>
@@ -1108,7 +1108,7 @@
       </c>
       <c r="D22" s="7"/>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="7" t="s">
         <v>112</v>
       </c>
@@ -1119,7 +1119,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="7" t="s">
         <v>107</v>
       </c>
@@ -1130,7 +1130,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="7" t="s">
         <v>108</v>
       </c>
@@ -1141,7 +1141,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="7" t="s">
         <v>109</v>
       </c>
@@ -1152,7 +1152,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" s="7" t="s">
         <v>110</v>
       </c>
@@ -1166,7 +1166,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" s="7" t="s">
         <v>29</v>
       </c>
@@ -1180,7 +1180,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" s="7" t="s">
         <v>105</v>
       </c>
@@ -1194,7 +1194,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" s="7" t="s">
         <v>30</v>
       </c>
@@ -1206,7 +1206,7 @@
       </c>
       <c r="D30" s="7"/>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" s="7" t="s">
         <v>31</v>
       </c>
@@ -1218,7 +1218,7 @@
       </c>
       <c r="D31" s="7"/>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
         <v>34</v>
       </c>
@@ -1232,7 +1232,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
         <v>35</v>
       </c>
@@ -1246,7 +1246,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
         <v>85</v>
       </c>
@@ -1260,7 +1260,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" s="10" t="s">
         <v>5</v>
       </c>
@@ -1272,7 +1272,7 @@
       </c>
       <c r="D35" s="10"/>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" s="10" t="s">
         <v>6</v>
       </c>
@@ -1284,7 +1284,7 @@
       </c>
       <c r="D36" s="10"/>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" s="10" t="s">
         <v>7</v>
       </c>
@@ -1296,7 +1296,7 @@
       </c>
       <c r="D37" s="10"/>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" s="10" t="s">
         <v>8</v>
       </c>
@@ -1308,7 +1308,7 @@
       </c>
       <c r="D38" s="10"/>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" s="10" t="s">
         <v>9</v>
       </c>
@@ -1320,7 +1320,7 @@
       </c>
       <c r="D39" s="10"/>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" s="10" t="s">
         <v>10</v>
       </c>
@@ -1332,7 +1332,7 @@
       </c>
       <c r="D40" s="10"/>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" s="10" t="s">
         <v>95</v>
       </c>
@@ -1346,7 +1346,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" s="10" t="s">
         <v>96</v>
       </c>
@@ -1360,7 +1360,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" s="10" t="s">
         <v>97</v>
       </c>
@@ -1374,7 +1374,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" s="3" t="s">
         <v>54</v>
       </c>
@@ -1386,7 +1386,7 @@
       </c>
       <c r="D44" s="3"/>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
         <v>28</v>
       </c>
@@ -1398,7 +1398,7 @@
       </c>
       <c r="D45" s="1"/>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
         <v>70</v>
       </c>
@@ -1410,7 +1410,7 @@
       </c>
       <c r="D46" s="1"/>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
         <v>25</v>
       </c>
@@ -1422,7 +1422,7 @@
       </c>
       <c r="D47" s="1"/>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
         <v>71</v>
       </c>
@@ -1434,7 +1434,7 @@
       </c>
       <c r="D48" s="1"/>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
         <v>26</v>
       </c>
@@ -1448,7 +1448,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
         <v>72</v>
       </c>
@@ -1462,7 +1462,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="51" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="51" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A51" s="1" t="s">
         <v>99</v>
       </c>
@@ -1474,7 +1474,7 @@
       </c>
       <c r="D51" s="1"/>
     </row>
-    <row r="52" spans="1:4" ht="15" thickTop="1" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:4" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A52" s="13" t="s">
         <v>32</v>
       </c>
@@ -1486,7 +1486,7 @@
       </c>
       <c r="D52" s="13"/>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53" s="5" t="s">
         <v>73</v>
       </c>
@@ -1498,7 +1498,7 @@
       </c>
       <c r="D53" s="5"/>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A54" s="5" t="s">
         <v>23</v>
       </c>
@@ -1512,7 +1512,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A55" s="5" t="s">
         <v>24</v>
       </c>
@@ -1526,7 +1526,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A56" s="5" t="s">
         <v>86</v>
       </c>
@@ -1540,7 +1540,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A57" s="5" t="s">
         <v>88</v>
       </c>
@@ -1554,7 +1554,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A58" s="5" t="s">
         <v>89</v>
       </c>
@@ -1568,7 +1568,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A59" s="8" t="s">
         <v>39</v>
       </c>
@@ -1582,7 +1582,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A60" s="6" t="s">
         <v>33</v>
       </c>
@@ -1596,7 +1596,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A61" s="6" t="s">
         <v>42</v>
       </c>
@@ -1608,7 +1608,7 @@
       </c>
       <c r="D61" s="6"/>
     </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A62" s="6" t="s">
         <v>47</v>
       </c>
@@ -1620,7 +1620,7 @@
       </c>
       <c r="D62" s="6"/>
     </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A63" s="6" t="s">
         <v>43</v>
       </c>
@@ -1632,7 +1632,7 @@
       </c>
       <c r="D63" s="6"/>
     </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A64" s="1" t="s">
         <v>48</v>
       </c>
@@ -1644,7 +1644,7 @@
       </c>
       <c r="D64" s="1"/>
     </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A65" s="4" t="s">
         <v>36</v>
       </c>
@@ -1656,7 +1656,7 @@
       </c>
       <c r="D65" s="4"/>
     </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A66" s="4" t="s">
         <v>38</v>
       </c>
@@ -1670,7 +1670,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A67" s="4" t="s">
         <v>44</v>
       </c>
@@ -1682,7 +1682,7 @@
       </c>
       <c r="D67" s="4"/>
     </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A68" s="7" t="s">
         <v>37</v>
       </c>
@@ -1694,7 +1694,7 @@
       </c>
       <c r="D68" s="7"/>
     </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A69" s="7" t="s">
         <v>56</v>
       </c>
@@ -1708,7 +1708,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A70" s="7" t="s">
         <v>55</v>
       </c>
@@ -1720,7 +1720,7 @@
       </c>
       <c r="D70" s="7"/>
     </row>
-    <row r="71" spans="1:4" ht="13.9" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:4" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A71" s="7" t="s">
         <v>81</v>
       </c>
@@ -1734,7 +1734,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="72" spans="1:4" ht="13.9" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:4" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A72" s="7" t="s">
         <v>82</v>
       </c>
@@ -1748,7 +1748,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A73" s="7" t="s">
         <v>83</v>
       </c>
@@ -1762,7 +1762,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A74" s="7" t="s">
         <v>63</v>
       </c>
@@ -1774,7 +1774,7 @@
       </c>
       <c r="D74" s="7"/>
     </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A75" s="7" t="s">
         <v>64</v>
       </c>
@@ -1788,7 +1788,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A76" s="7" t="s">
         <v>91</v>
       </c>
@@ -1802,7 +1802,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A77" s="7" t="s">
         <v>93</v>
       </c>
@@ -1816,7 +1816,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A78" s="7" t="s">
         <v>94</v>
       </c>
@@ -1830,7 +1830,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A79" s="7" t="s">
         <v>116</v>
       </c>
@@ -1844,7 +1844,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A80" s="7" t="s">
         <v>118</v>
       </c>
@@ -1893,9 +1893,9 @@
       <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>46</v>
       </c>
@@ -1906,7 +1906,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>58</v>
       </c>
@@ -1917,7 +1917,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>59</v>
       </c>
@@ -1928,7 +1928,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>79</v>
       </c>
@@ -1936,7 +1936,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>80</v>
       </c>

</xml_diff>

<commit_message>
New TB NH params
</commit_message>
<xml_diff>
--- a/spreadsheets/common_parameters.xlsx
+++ b/spreadsheets/common_parameters.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20344"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20346"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rrag0004\Models\SNAP-TB_new\spreadsheets\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rrag0004\Models\SNAP_TB_BMC_MED\spreadsheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4E2BBB8-269C-4936-A5E5-D6A9FC7F4723}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A40B98C-0AF1-4EE3-9FC9-F3A71E568EC2}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="16395" windowHeight="6600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="207" uniqueCount="115">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="232" uniqueCount="125">
   <si>
     <t>float</t>
   </si>
@@ -79,6 +79,9 @@
     <t>active_age_low</t>
   </si>
   <si>
+    <t>active_age_high</t>
+  </si>
+  <si>
     <t>perc_active</t>
   </si>
   <si>
@@ -100,18 +103,27 @@
     <t>perc_treatment_success</t>
   </si>
   <si>
-    <t>!!! Unit Year-1</t>
+    <t>perc_sp_cure_smearpos</t>
+  </si>
+  <si>
+    <t>lambda_timeto_sp_or_death_smearpos</t>
   </si>
   <si>
     <t>perc_smearpos</t>
   </si>
   <si>
+    <t>minimal_age_infectious</t>
+  </si>
+  <si>
     <t>rel_infectiousness_after_detect</t>
   </si>
   <si>
     <t>rel_infectiousness_smearneg</t>
   </si>
   <si>
+    <t>perc_cdr_smearpos</t>
+  </si>
+  <si>
     <t>pt_efficacy</t>
   </si>
   <si>
@@ -214,6 +226,9 @@
     <t>none</t>
   </si>
   <si>
+    <t>active TB</t>
+  </si>
+  <si>
     <t>absolute number of TB cases</t>
   </si>
   <si>
@@ -223,6 +238,15 @@
     <t>perc_extrapulmonary</t>
   </si>
   <si>
+    <t>perc_sp_cure_closed_tb</t>
+  </si>
+  <si>
+    <t>lambda_timeto_sp_or_death_closed_tb</t>
+  </si>
+  <si>
+    <t>perc_cdr_closed_tb</t>
+  </si>
+  <si>
     <t>sd_agepreference_school</t>
   </si>
   <si>
@@ -316,6 +340,12 @@
     <t>average nb of potential contacts at work</t>
   </si>
   <si>
+    <t>age_maximal_infectiousness_reached</t>
+  </si>
+  <si>
+    <t>NOT USED</t>
+  </si>
+  <si>
     <t>prop_physical_school_contact</t>
   </si>
   <si>
@@ -349,38 +379,46 @@
     <t>age at which infectiousness multiplier reaches .5</t>
   </si>
   <si>
-    <t>percentage. Only used in absence of time-variant data</t>
-  </si>
-  <si>
-    <t>normally replaced with time-variant</t>
-  </si>
-  <si>
-    <t>rate_self_cure_smearpos</t>
-  </si>
-  <si>
-    <t>rate_self_cure_closed_tb</t>
+    <t>tb_mortality_multiplier</t>
+  </si>
+  <si>
+    <t>old tbnh params</t>
+  </si>
+  <si>
+    <t>!!! Unit Year-1     old tbnh params</t>
+  </si>
+  <si>
+    <t>rate_sp_cure_smearpos</t>
+  </si>
+  <si>
+    <t>rate_sp_cure_closed_tb</t>
   </si>
   <si>
     <t>rate_tb_mortality_smearpos</t>
   </si>
   <si>
+    <t>year-1   new tbnh params</t>
+  </si>
+  <si>
     <t>rate_tb_mortality_closed_tb</t>
-  </si>
-  <si>
-    <t>perc_cdr</t>
-  </si>
-  <si>
-    <t>only used in absence of time-variant data</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -467,7 +505,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="-0.249977111117893"/>
+        <fgColor theme="2" tint="-0.499984740745262"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -493,7 +531,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -509,6 +547,7 @@
     <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="11" fontId="0" fillId="11" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="14" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
@@ -791,22 +830,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D75"/>
+  <dimension ref="A1:D84"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A64" zoomScale="205" zoomScaleNormal="205" workbookViewId="0">
-      <selection activeCell="A74" sqref="A74"/>
+    <sheetView tabSelected="1" topLeftCell="A28" zoomScale="205" zoomScaleNormal="205" workbookViewId="0">
+      <selection activeCell="B32" sqref="B32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="44" customWidth="1"/>
-    <col min="2" max="2" width="16" customWidth="1"/>
+    <col min="1" max="1" width="37.7109375" customWidth="1"/>
+    <col min="2" max="2" width="11.7109375" customWidth="1"/>
     <col min="4" max="4" width="65.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="10" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="B1" s="10">
         <v>10000</v>
@@ -832,7 +871,7 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="11" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="B3" s="11">
         <v>18</v>
@@ -844,7 +883,7 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="11" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="B4" s="11">
         <v>30</v>
@@ -856,7 +895,7 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="11" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="B5" s="11">
         <v>10</v>
@@ -865,7 +904,7 @@
         <v>0</v>
       </c>
       <c r="D5" s="11" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -897,206 +936,209 @@
         <v>17</v>
       </c>
       <c r="B8" s="11">
-        <v>60</v>
+        <v>65</v>
       </c>
       <c r="C8" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="D8" s="11" t="s">
-        <v>18</v>
+      <c r="D8" s="15" t="s">
+        <v>105</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="11" t="s">
-        <v>48</v>
+        <v>18</v>
       </c>
       <c r="B9" s="11">
-        <v>0</v>
+        <v>60</v>
       </c>
       <c r="C9" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="D9" s="11"/>
+      <c r="D9" s="11" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="9" t="s">
-        <v>93</v>
-      </c>
-      <c r="B10" s="9">
-        <v>200</v>
-      </c>
-      <c r="C10" s="9" t="s">
-        <v>0</v>
-      </c>
-      <c r="D10" s="9" t="s">
-        <v>94</v>
-      </c>
+      <c r="A10" s="11" t="s">
+        <v>52</v>
+      </c>
+      <c r="B10" s="11">
+        <v>0</v>
+      </c>
+      <c r="C10" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="D10" s="11"/>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="9" t="s">
-        <v>92</v>
+        <v>101</v>
       </c>
       <c r="B11" s="9">
-        <v>20</v>
+        <v>200</v>
       </c>
       <c r="C11" s="9" t="s">
         <v>0</v>
       </c>
       <c r="D11" s="9" t="s">
-        <v>95</v>
+        <v>102</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="9" t="s">
-        <v>19</v>
+        <v>100</v>
       </c>
       <c r="B12" s="9">
-        <v>100</v>
+        <v>20</v>
       </c>
       <c r="C12" s="9" t="s">
         <v>0</v>
       </c>
       <c r="D12" s="9" t="s">
-        <v>20</v>
+        <v>103</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="9" t="s">
-        <v>65</v>
+        <v>20</v>
       </c>
       <c r="B13" s="9">
-        <v>2</v>
+        <v>100</v>
       </c>
       <c r="C13" s="9" t="s">
         <v>0</v>
       </c>
       <c r="D13" s="9" t="s">
-        <v>67</v>
+        <v>21</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="9" t="s">
-        <v>66</v>
+        <v>73</v>
       </c>
       <c r="B14" s="9">
+        <v>2</v>
+      </c>
+      <c r="C14" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="D14" s="9" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" s="9" t="s">
+        <v>74</v>
+      </c>
+      <c r="B15" s="9">
         <v>10</v>
       </c>
-      <c r="C14" s="9" t="s">
-        <v>0</v>
-      </c>
-      <c r="D14" s="9" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="14" t="s">
-        <v>69</v>
-      </c>
-      <c r="B15" s="14">
+      <c r="C15" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="D15" s="9" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="14" t="s">
+        <v>77</v>
+      </c>
+      <c r="B16" s="14">
         <v>15.5</v>
       </c>
-      <c r="C15" s="14" t="s">
-        <v>0</v>
-      </c>
-      <c r="D15" s="14" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="12" t="s">
+      <c r="C16" s="14" t="s">
+        <v>0</v>
+      </c>
+      <c r="D16" s="14" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="B16" s="12">
+      <c r="B17" s="12">
         <v>95</v>
       </c>
-      <c r="C16" s="12" t="s">
-        <v>0</v>
-      </c>
-      <c r="D16" s="12" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" s="7" t="s">
-        <v>102</v>
-      </c>
-      <c r="B17" s="7">
-        <v>0.7</v>
-      </c>
-      <c r="C17" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="D17" s="7"/>
+      <c r="C17" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="D17" s="12" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="7" t="s">
-        <v>103</v>
+        <v>112</v>
       </c>
       <c r="B18" s="7">
-        <v>15</v>
+        <v>0.7</v>
       </c>
       <c r="C18" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="D18" s="7" t="s">
-        <v>35</v>
-      </c>
+      <c r="D18" s="7"/>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="7" t="s">
-        <v>104</v>
+        <v>113</v>
       </c>
       <c r="B19" s="7">
-        <v>30</v>
+        <v>15</v>
       </c>
       <c r="C19" s="7" t="s">
         <v>0</v>
       </c>
       <c r="D19" s="7" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="B20" s="7" t="b">
-        <v>1</v>
+        <v>114</v>
+      </c>
+      <c r="B20" s="7">
+        <v>30</v>
       </c>
       <c r="C20" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="D20" s="7"/>
+        <v>0</v>
+      </c>
+      <c r="D20" s="7" t="s">
+        <v>39</v>
+      </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="B21" s="7">
-        <v>3.0000000000000001E-3</v>
+        <v>11</v>
+      </c>
+      <c r="B21" s="7" t="b">
+        <v>1</v>
       </c>
       <c r="C21" s="7" t="s">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="D21" s="7"/>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="7" t="s">
-        <v>101</v>
+        <v>13</v>
       </c>
       <c r="B22" s="7">
-        <v>0.75</v>
+        <v>3.0000000000000001E-3</v>
       </c>
       <c r="C22" s="7" t="s">
         <v>0</v>
       </c>
+      <c r="D22" s="7"/>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="7" t="s">
-        <v>96</v>
+        <v>111</v>
       </c>
       <c r="B23" s="7">
-        <v>0.5</v>
+        <v>0.75</v>
       </c>
       <c r="C23" s="7" t="s">
         <v>0</v>
@@ -1104,10 +1146,10 @@
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="7" t="s">
-        <v>97</v>
+        <v>106</v>
       </c>
       <c r="B24" s="7">
-        <v>0.34</v>
+        <v>0.5</v>
       </c>
       <c r="C24" s="7" t="s">
         <v>0</v>
@@ -1115,10 +1157,10 @@
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="7" t="s">
-        <v>98</v>
+        <v>107</v>
       </c>
       <c r="B25" s="7">
-        <v>0.45</v>
+        <v>0.34</v>
       </c>
       <c r="C25" s="7" t="s">
         <v>0</v>
@@ -1126,126 +1168,129 @@
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="7" t="s">
-        <v>99</v>
+        <v>108</v>
       </c>
       <c r="B26" s="7">
-        <v>0.5</v>
+        <v>0.45</v>
       </c>
       <c r="C26" s="7" t="s">
         <v>0</v>
-      </c>
-      <c r="D26" t="s">
-        <v>100</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" s="7" t="s">
-        <v>26</v>
+        <v>109</v>
       </c>
       <c r="B27" s="7">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="C27" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="D27" s="7"/>
+      <c r="D27" t="s">
+        <v>110</v>
+      </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" s="7" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B28" s="7">
+        <v>10</v>
+      </c>
+      <c r="C28" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="D28" s="15" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29" s="7" t="s">
+        <v>104</v>
+      </c>
+      <c r="B29" s="7">
+        <v>15</v>
+      </c>
+      <c r="C29" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="D29" s="15" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="B30" s="7">
+        <v>0.5</v>
+      </c>
+      <c r="C30" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="D30" s="7"/>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A31" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="B31" s="7">
         <v>0.25</v>
       </c>
-      <c r="C28" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="D28" s="7"/>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A29" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="B29" s="2">
+      <c r="C31" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="D31" s="7"/>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A32" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B32" s="2">
         <v>20</v>
       </c>
-      <c r="C29" s="2" t="s">
+      <c r="C32" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="D29" s="2" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A30" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="B30" s="2">
-        <v>0</v>
-      </c>
-      <c r="C30" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="D30" s="2" t="s">
+      <c r="D32" s="2" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A33" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B33" s="2">
+        <v>0</v>
+      </c>
+      <c r="C33" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="D33" s="2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A31" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="B31" s="2">
-        <v>0</v>
-      </c>
-      <c r="C31" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="D31" s="2" t="s">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A34" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="B34" s="2">
+        <v>0</v>
+      </c>
+      <c r="C34" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="D34" s="2" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A32" s="10" t="s">
-        <v>5</v>
-      </c>
-      <c r="B32" s="15">
-        <v>1.9E-2</v>
-      </c>
-      <c r="C32" s="10" t="s">
-        <v>0</v>
-      </c>
-      <c r="D32" s="10"/>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A33" s="10" t="s">
-        <v>6</v>
-      </c>
-      <c r="B33" s="15">
-        <v>1.4E-2</v>
-      </c>
-      <c r="C33" s="10" t="s">
-        <v>0</v>
-      </c>
-      <c r="D33" s="10"/>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A34" s="10" t="s">
-        <v>7</v>
-      </c>
-      <c r="B34" s="15">
-        <v>5.5999999999999999E-3</v>
-      </c>
-      <c r="C34" s="10" t="s">
-        <v>0</v>
-      </c>
-      <c r="D34" s="10"/>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" s="10" t="s">
-        <v>8</v>
-      </c>
-      <c r="B35" s="15">
-        <v>3.3999999999999999E-11</v>
+        <v>5</v>
+      </c>
+      <c r="B35" s="16">
+        <v>1.9E-2</v>
       </c>
       <c r="C35" s="10" t="s">
         <v>0</v>
@@ -1254,10 +1299,10 @@
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="B36" s="15">
-        <v>6.3999999999999997E-6</v>
+        <v>6</v>
+      </c>
+      <c r="B36" s="16">
+        <v>1.4E-2</v>
       </c>
       <c r="C36" s="10" t="s">
         <v>0</v>
@@ -1266,10 +1311,10 @@
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="B37" s="15">
-        <v>3.3000000000000002E-6</v>
+        <v>7</v>
+      </c>
+      <c r="B37" s="16">
+        <v>5.5999999999999999E-3</v>
       </c>
       <c r="C37" s="10" t="s">
         <v>0</v>
@@ -1278,102 +1323,100 @@
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" s="10" t="s">
-        <v>86</v>
-      </c>
-      <c r="B38" s="10">
-        <v>0.65</v>
+        <v>8</v>
+      </c>
+      <c r="B38" s="16">
+        <v>3.3999999999999999E-11</v>
       </c>
       <c r="C38" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="D38" s="10" t="s">
-        <v>89</v>
-      </c>
+      <c r="D38" s="10"/>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" s="10" t="s">
-        <v>87</v>
-      </c>
-      <c r="B39" s="10">
-        <v>0.81</v>
+        <v>9</v>
+      </c>
+      <c r="B39" s="16">
+        <v>6.3999999999999997E-6</v>
       </c>
       <c r="C39" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="D39" s="10" t="s">
-        <v>89</v>
-      </c>
+      <c r="D39" s="10"/>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" s="10" t="s">
-        <v>88</v>
-      </c>
-      <c r="B40" s="10">
+        <v>10</v>
+      </c>
+      <c r="B40" s="16">
+        <v>3.3000000000000002E-6</v>
+      </c>
+      <c r="C40" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="D40" s="10"/>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A41" s="10" t="s">
+        <v>94</v>
+      </c>
+      <c r="B41" s="10">
+        <v>0.65</v>
+      </c>
+      <c r="C41" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="D41" s="10" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A42" s="10" t="s">
+        <v>95</v>
+      </c>
+      <c r="B42" s="10">
+        <v>0.81</v>
+      </c>
+      <c r="C42" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="D42" s="10" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A43" s="10" t="s">
+        <v>96</v>
+      </c>
+      <c r="B43" s="10">
         <v>0.95</v>
       </c>
-      <c r="C40" s="10" t="s">
-        <v>0</v>
-      </c>
-      <c r="D40" s="10" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A41" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="B41" s="3" t="b">
-        <v>0</v>
-      </c>
-      <c r="C41" s="3" t="s">
+      <c r="C43" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="D43" s="10" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A44" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="B44" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="C44" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="D41" s="3"/>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A42" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="B42" s="1">
-        <v>50</v>
-      </c>
-      <c r="C42" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D42" s="1" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A43" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="B43" s="1">
-        <v>25</v>
-      </c>
-      <c r="C43" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D43" s="1"/>
-    </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A44" s="1" t="s">
-        <v>109</v>
-      </c>
-      <c r="B44" s="1">
-        <v>0.23300000000000001</v>
-      </c>
-      <c r="C44" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D44" s="1"/>
+      <c r="D44" s="3"/>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
-        <v>110</v>
+        <v>27</v>
       </c>
       <c r="B45" s="1">
-        <v>0.14699999999999999</v>
+        <v>50</v>
       </c>
       <c r="C45" s="1" t="s">
         <v>0</v>
@@ -1382,402 +1425,519 @@
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
-        <v>111</v>
+        <v>69</v>
       </c>
       <c r="B46" s="1">
+        <v>25</v>
+      </c>
+      <c r="C46" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D46" s="1"/>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A47" s="17" t="s">
+        <v>25</v>
+      </c>
+      <c r="B47" s="17">
+        <v>27</v>
+      </c>
+      <c r="C47" s="17" t="s">
+        <v>0</v>
+      </c>
+      <c r="D47" s="17" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A48" s="17" t="s">
+        <v>70</v>
+      </c>
+      <c r="B48" s="17">
+        <v>52</v>
+      </c>
+      <c r="C48" s="17" t="s">
+        <v>0</v>
+      </c>
+      <c r="D48" s="17" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A49" s="17" t="s">
+        <v>26</v>
+      </c>
+      <c r="B49" s="17">
+        <v>0.33600000000000002</v>
+      </c>
+      <c r="C49" s="17" t="s">
+        <v>0</v>
+      </c>
+      <c r="D49" s="17" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A50" s="17" t="s">
+        <v>71</v>
+      </c>
+      <c r="B50" s="17">
+        <v>5.8000000000000003E-2</v>
+      </c>
+      <c r="C50" s="17" t="s">
+        <v>0</v>
+      </c>
+      <c r="D50" s="17" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A51" s="6" t="s">
+        <v>120</v>
+      </c>
+      <c r="B51" s="6">
+        <v>0.23300000000000001</v>
+      </c>
+      <c r="C51" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="D51" s="6" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A52" s="6" t="s">
+        <v>121</v>
+      </c>
+      <c r="B52" s="6">
+        <v>0.14699999999999999</v>
+      </c>
+      <c r="C52" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="D52" s="6" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A53" s="6" t="s">
+        <v>122</v>
+      </c>
+      <c r="B53" s="6">
         <v>0.39</v>
       </c>
-      <c r="C46" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D46" s="1" t="s">
+      <c r="C53" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="D53" s="6" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A54" s="6" t="s">
+        <v>124</v>
+      </c>
+      <c r="B54" s="6">
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="C54" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="D54" s="6" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A55" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="B55" s="1">
+        <v>0.21</v>
+      </c>
+      <c r="C55" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D55" s="1"/>
+    </row>
+    <row r="56" spans="1:4" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A56" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="B56" s="13">
+        <v>77</v>
+      </c>
+      <c r="C56" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="D56" s="13"/>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A57" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="B57" s="5">
+        <v>77</v>
+      </c>
+      <c r="C57" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="D57" s="5"/>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A58" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="B58" s="5">
+        <v>7</v>
+      </c>
+      <c r="C58" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="D58" s="5" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A59" s="5" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A47" s="1" t="s">
-        <v>112</v>
-      </c>
-      <c r="B47" s="1">
-        <v>2.5000000000000001E-2</v>
-      </c>
-      <c r="C47" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D47" s="1" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="48" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A48" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="B48" s="1">
-        <v>0.21</v>
-      </c>
-      <c r="C48" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D48" s="1"/>
-    </row>
-    <row r="49" spans="1:4" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="13" t="s">
-        <v>113</v>
-      </c>
-      <c r="B49" s="13">
-        <v>77</v>
-      </c>
-      <c r="C49" s="13" t="s">
-        <v>0</v>
-      </c>
-      <c r="D49" s="13" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A50" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="B50" s="5">
-        <v>7</v>
-      </c>
-      <c r="C50" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="D50" s="5" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A51" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="B51" s="5">
+      <c r="B59" s="5">
         <v>92</v>
       </c>
-      <c r="C51" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="D51" s="5" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A52" s="16" t="s">
-        <v>77</v>
-      </c>
-      <c r="B52" s="16">
+      <c r="C59" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="D59" s="5" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A60" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="B60" s="5">
         <v>0.6</v>
       </c>
-      <c r="C52" s="16" t="s">
-        <v>0</v>
-      </c>
-      <c r="D52" s="16" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A53" s="16" t="s">
-        <v>79</v>
-      </c>
-      <c r="B53" s="16">
+      <c r="C60" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="D60" s="5" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A61" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="B61" s="5">
         <v>50</v>
       </c>
-      <c r="C53" s="16" t="s">
-        <v>0</v>
-      </c>
-      <c r="D53" s="16" t="s">
+      <c r="C61" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="D61" s="5" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A54" s="16" t="s">
-        <v>80</v>
-      </c>
-      <c r="B54" s="16">
-        <v>0</v>
-      </c>
-      <c r="C54" s="16" t="s">
-        <v>0</v>
-      </c>
-      <c r="D54" s="16" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A55" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="B55" s="8">
-        <v>0</v>
-      </c>
-      <c r="C55" s="8" t="s">
-        <v>0</v>
-      </c>
-      <c r="D55" s="8" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A56" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="B56" s="6">
+    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A62" s="5" t="s">
+        <v>88</v>
+      </c>
+      <c r="B62" s="5">
+        <v>0</v>
+      </c>
+      <c r="C62" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="D62" s="5" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A63" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="B63" s="8">
+        <v>0</v>
+      </c>
+      <c r="C63" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="D63" s="8" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A64" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="B64" s="6">
         <v>0.6</v>
       </c>
-      <c r="C56" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="D56" s="6" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A57" s="6" t="s">
+      <c r="C64" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="D64" s="6" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A65" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="B65" s="6">
+        <v>0.84</v>
+      </c>
+      <c r="C65" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="D65" s="6"/>
+    </row>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A66" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="B66" s="6">
+        <v>0.95</v>
+      </c>
+      <c r="C66" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="D66" s="6"/>
+    </row>
+    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A67" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="B67" s="6">
+        <v>0.8</v>
+      </c>
+      <c r="C67" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="D67" s="6"/>
+    </row>
+    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A68" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B68" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="C68" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D68" s="1"/>
+    </row>
+    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A69" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="B69" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="C69" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D69" s="4"/>
+    </row>
+    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A70" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="B57" s="6">
-        <v>0.84</v>
-      </c>
-      <c r="C57" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="D57" s="6"/>
-    </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A58" s="6" t="s">
-        <v>42</v>
-      </c>
-      <c r="B58" s="6">
-        <v>0.95</v>
-      </c>
-      <c r="C58" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="D58" s="6"/>
-    </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A59" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="B59" s="6">
-        <v>0.8</v>
-      </c>
-      <c r="C59" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="D59" s="6"/>
-    </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A60" s="1" t="s">
+      <c r="B70" s="4">
+        <v>10</v>
+      </c>
+      <c r="C70" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="D70" s="4" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A71" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="B60" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="C60" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="D60" s="1"/>
-    </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A61" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="B61" s="4" t="b">
-        <v>0</v>
-      </c>
-      <c r="C61" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="D61" s="4"/>
-    </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A62" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="B62" s="4">
-        <v>10</v>
-      </c>
-      <c r="C62" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="D62" s="4" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A63" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="B63" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="C63" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="D63" s="4"/>
-    </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A64" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="B64" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="C64" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="D64" s="7"/>
-    </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A65" s="7" t="s">
-        <v>51</v>
-      </c>
-      <c r="B65" s="7" t="s">
-        <v>41</v>
-      </c>
-      <c r="C65" s="7" t="s">
-        <v>40</v>
-      </c>
-      <c r="D65" s="7" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A66" s="7" t="s">
-        <v>50</v>
-      </c>
-      <c r="B66" s="7" t="s">
-        <v>56</v>
-      </c>
-      <c r="C66" s="7" t="s">
-        <v>40</v>
-      </c>
-      <c r="D66" s="7"/>
-    </row>
-    <row r="67" spans="1:4" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A67" s="7" t="s">
-        <v>72</v>
-      </c>
-      <c r="B67" s="7">
-        <v>0</v>
-      </c>
-      <c r="C67" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="D67" s="7" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="68" spans="1:4" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A68" s="7" t="s">
-        <v>73</v>
-      </c>
-      <c r="B68" s="7">
-        <v>0</v>
-      </c>
-      <c r="C68" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="D68" s="7" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A69" s="7" t="s">
-        <v>74</v>
-      </c>
-      <c r="B69" s="7">
-        <v>0</v>
-      </c>
-      <c r="C69" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="D69" s="7" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A70" s="7" t="s">
-        <v>58</v>
-      </c>
-      <c r="B70" s="7" t="s">
-        <v>41</v>
-      </c>
-      <c r="C70" s="7" t="s">
-        <v>40</v>
-      </c>
-      <c r="D70" s="7"/>
-    </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A71" s="7" t="s">
-        <v>59</v>
-      </c>
-      <c r="B71" s="7">
-        <v>7</v>
-      </c>
-      <c r="C71" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="D71" s="7" t="s">
-        <v>60</v>
-      </c>
+      <c r="B71" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="C71" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="D71" s="4"/>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A72" s="7" t="s">
-        <v>82</v>
-      </c>
-      <c r="B72" s="7">
-        <v>100</v>
+        <v>36</v>
+      </c>
+      <c r="B72" s="7" t="b">
+        <v>0</v>
       </c>
       <c r="C72" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="D72" s="7" t="s">
-        <v>83</v>
-      </c>
+        <v>12</v>
+      </c>
+      <c r="D72" s="7"/>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A73" s="7" t="s">
-        <v>84</v>
-      </c>
-      <c r="B73" s="7">
-        <v>50</v>
+        <v>55</v>
+      </c>
+      <c r="B73" s="7" t="s">
+        <v>45</v>
       </c>
       <c r="C73" s="7" t="s">
-        <v>0</v>
+        <v>44</v>
       </c>
       <c r="D73" s="7" t="s">
-        <v>83</v>
+        <v>56</v>
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A74" s="7" t="s">
-        <v>85</v>
-      </c>
-      <c r="B74" s="7">
+        <v>54</v>
+      </c>
+      <c r="B74" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="C74" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="D74" s="7"/>
+    </row>
+    <row r="75" spans="1:4" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A75" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="B75" s="7">
+        <v>0</v>
+      </c>
+      <c r="C75" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="D75" s="7" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="76" spans="1:4" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A76" s="7" t="s">
+        <v>81</v>
+      </c>
+      <c r="B76" s="7">
+        <v>0</v>
+      </c>
+      <c r="C76" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="D76" s="7" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A77" s="7" t="s">
+        <v>82</v>
+      </c>
+      <c r="B77" s="7">
+        <v>0</v>
+      </c>
+      <c r="C77" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="D77" s="7" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A78" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="B78" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="C78" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="D78" s="7"/>
+    </row>
+    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A79" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="B79" s="7">
+        <v>7</v>
+      </c>
+      <c r="C79" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="D79" s="7" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A80" s="7" t="s">
+        <v>90</v>
+      </c>
+      <c r="B80" s="7">
+        <v>100</v>
+      </c>
+      <c r="C80" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="D80" s="7" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A81" s="7" t="s">
+        <v>92</v>
+      </c>
+      <c r="B81" s="7">
+        <v>50</v>
+      </c>
+      <c r="C81" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="D81" s="7" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A82" s="7" t="s">
+        <v>93</v>
+      </c>
+      <c r="B82" s="7">
         <v>150</v>
       </c>
-      <c r="C74" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="D74" s="7" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A75" s="7" t="s">
-        <v>105</v>
-      </c>
-      <c r="B75" s="7">
+      <c r="C82" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="D82" s="7" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A83" s="7" t="s">
+        <v>115</v>
+      </c>
+      <c r="B83" s="7">
         <v>15</v>
       </c>
-      <c r="C75" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="D75" s="7" t="s">
-        <v>106</v>
+      <c r="C83" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="D83" s="7" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A84" s="7" t="s">
+        <v>117</v>
+      </c>
+      <c r="B84" s="7">
+        <v>1</v>
+      </c>
+      <c r="C84" s="7" t="s">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -1790,19 +1950,19 @@
           <x14:formula1>
             <xm:f>dropdown!$C$1:$C$3</xm:f>
           </x14:formula1>
-          <xm:sqref>B63 B66</xm:sqref>
+          <xm:sqref>B71 B74</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-000001000000}">
           <x14:formula1>
             <xm:f>dropdown!$A$1:$A$5</xm:f>
           </x14:formula1>
-          <xm:sqref>B65</xm:sqref>
+          <xm:sqref>B73</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-000002000000}">
           <x14:formula1>
             <xm:f>dropdown!$E$1:$E$5</xm:f>
           </x14:formula1>
-          <xm:sqref>B70</xm:sqref>
+          <xm:sqref>B78</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -1822,51 +1982,51 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>41</v>
+        <v>45</v>
       </c>
       <c r="C1" t="s">
-        <v>41</v>
+        <v>45</v>
       </c>
       <c r="E1" t="s">
-        <v>41</v>
+        <v>45</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="C2" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="E2" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="C3" t="s">
-        <v>56</v>
+        <v>60</v>
       </c>
       <c r="E3" t="s">
-        <v>56</v>
+        <v>60</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>70</v>
+        <v>78</v>
       </c>
       <c r="E4" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>71</v>
+        <v>79</v>
       </c>
       <c r="E5" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
clean previous prevalence targeting
</commit_message>
<xml_diff>
--- a/spreadsheets/common_parameters.xlsx
+++ b/spreadsheets/common_parameters.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rrag0004\Models\SNAP-TB_new\spreadsheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{540AE985-519C-4699-AAD2-381069B43509}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F3172DA-22D9-41D1-883D-FFE0C3E49DCE}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="16395" windowHeight="6600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="222" uniqueCount="121">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="213" uniqueCount="117">
   <si>
     <t>float</t>
   </si>
@@ -290,18 +290,6 @@
   </si>
   <si>
     <t>percentage. Among unsuccesful treatments.</t>
-  </si>
-  <si>
-    <t>targetted_prevalence</t>
-  </si>
-  <si>
-    <t>/100K population</t>
-  </si>
-  <si>
-    <t>targetted_prevalence_low</t>
-  </si>
-  <si>
-    <t>targetted_prevalence_high</t>
   </si>
   <si>
     <t>g_child</t>
@@ -811,10 +799,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D80"/>
+  <dimension ref="A1:D77"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A70" zoomScale="205" zoomScaleNormal="205" workbookViewId="0">
-      <selection activeCell="A80" sqref="A80"/>
+      <selection activeCell="A75" sqref="A75"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -923,7 +911,7 @@
         <v>0</v>
       </c>
       <c r="D8" s="14" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
@@ -954,7 +942,7 @@
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="8" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="B11" s="8">
         <v>200</v>
@@ -963,12 +951,12 @@
         <v>0</v>
       </c>
       <c r="D11" s="8" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="8" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="B12" s="8">
         <v>20</v>
@@ -977,7 +965,7 @@
         <v>0</v>
       </c>
       <c r="D12" s="8" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
@@ -1052,7 +1040,7 @@
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="6" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="B18" s="6">
         <v>0.7</v>
@@ -1064,7 +1052,7 @@
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="6" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="B19" s="6">
         <v>15</v>
@@ -1078,7 +1066,7 @@
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="6" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="B20" s="6">
         <v>30</v>
@@ -1116,7 +1104,7 @@
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="6" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="B23" s="6">
         <v>0.75</v>
@@ -1127,7 +1115,7 @@
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="6" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="B24" s="6">
         <v>0.5</v>
@@ -1138,7 +1126,7 @@
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="6" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="B25" s="6">
         <v>0.34</v>
@@ -1149,7 +1137,7 @@
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="6" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="B26" s="6">
         <v>0.45</v>
@@ -1160,7 +1148,7 @@
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" s="6" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="B27" s="6">
         <v>0.5</v>
@@ -1169,7 +1157,7 @@
         <v>0</v>
       </c>
       <c r="D27" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
@@ -1312,7 +1300,7 @@
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" s="9" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="B39" s="9">
         <v>0.65</v>
@@ -1321,12 +1309,12 @@
         <v>0</v>
       </c>
       <c r="D39" s="9" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" s="9" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="B40" s="9">
         <v>0.81</v>
@@ -1335,12 +1323,12 @@
         <v>0</v>
       </c>
       <c r="D40" s="9" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" s="9" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="B41" s="9">
         <v>0.95</v>
@@ -1349,7 +1337,7 @@
         <v>0</v>
       </c>
       <c r="D41" s="9" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
@@ -1387,7 +1375,7 @@
         <v>0</v>
       </c>
       <c r="D44" s="16" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
@@ -1401,7 +1389,7 @@
         <v>0</v>
       </c>
       <c r="D45" s="16" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
@@ -1415,7 +1403,7 @@
         <v>0</v>
       </c>
       <c r="D46" s="16" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
@@ -1429,12 +1417,12 @@
         <v>0</v>
       </c>
       <c r="D47" s="16" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" s="5" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="B48" s="5">
         <v>0.23300000000000001</v>
@@ -1443,12 +1431,12 @@
         <v>0</v>
       </c>
       <c r="D48" s="5" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49" s="5" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="B49" s="5">
         <v>0.14699999999999999</v>
@@ -1457,12 +1445,12 @@
         <v>0</v>
       </c>
       <c r="D49" s="5" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50" s="5" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="B50" s="5">
         <v>0.39</v>
@@ -1471,12 +1459,12 @@
         <v>0</v>
       </c>
       <c r="D50" s="5" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51" s="5" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="B51" s="5">
         <v>2.5000000000000001E-2</v>
@@ -1485,12 +1473,12 @@
         <v>0</v>
       </c>
       <c r="D51" s="5" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
     </row>
     <row r="52" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A52" s="1" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="B52" s="1">
         <v>0.21</v>
@@ -1605,7 +1593,7 @@
         <v>0</v>
       </c>
       <c r="D60" s="7" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.25">
@@ -1816,58 +1804,16 @@
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A77" s="6" t="s">
-        <v>88</v>
+        <v>108</v>
       </c>
       <c r="B77" s="6">
-        <v>100</v>
+        <v>15</v>
       </c>
       <c r="C77" s="6" t="s">
         <v>0</v>
       </c>
       <c r="D77" s="6" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A78" s="6" t="s">
-        <v>90</v>
-      </c>
-      <c r="B78" s="6">
-        <v>50</v>
-      </c>
-      <c r="C78" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="D78" s="6" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A79" s="6" t="s">
-        <v>91</v>
-      </c>
-      <c r="B79" s="6">
-        <v>150</v>
-      </c>
-      <c r="C79" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="D79" s="6" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A80" s="6" t="s">
-        <v>112</v>
-      </c>
-      <c r="B80" s="6">
-        <v>15</v>
-      </c>
-      <c r="C80" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="D80" s="6" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Use standard config for testing
</commit_message>
<xml_diff>
--- a/spreadsheets/common_parameters.xlsx
+++ b/spreadsheets/common_parameters.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20346"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20352"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rrag0004\Models\SNAP_TB_BMC_MED\spreadsheets\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rrag0004\Models\SNAP-TB\spreadsheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A40B98C-0AF1-4EE3-9FC9-F3A71E568EC2}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB28D45F-7685-4E04-B9EE-B833A10C8AF1}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="16395" windowHeight="6600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -832,8 +832,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D84"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" zoomScale="205" zoomScaleNormal="205" workbookViewId="0">
-      <selection activeCell="B32" sqref="B32"/>
+    <sheetView tabSelected="1" topLeftCell="A70" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="C82" sqref="C82"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -848,7 +848,7 @@
         <v>48</v>
       </c>
       <c r="B1" s="10">
-        <v>10000</v>
+        <v>1000</v>
       </c>
       <c r="C1" s="10" t="s">
         <v>1</v>

</xml_diff>

<commit_message>
Remove unused parameter for retirement home
</commit_message>
<xml_diff>
--- a/spreadsheets/common_parameters.xlsx
+++ b/spreadsheets/common_parameters.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rrag0004\Models\SNAP-TB\spreadsheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{017148EE-E452-4014-A86E-16ED70146017}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C28166B9-F30C-4BA2-BD6A-FECAAF51D2B5}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="16395" windowHeight="6600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="230" uniqueCount="124">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="228" uniqueCount="123">
   <si>
     <t>float</t>
   </si>
@@ -182,9 +182,6 @@
   </si>
   <si>
     <t>duration_hh_eligible_for_birth</t>
-  </si>
-  <si>
-    <t>perc_single_over90yo_in_retirement_home</t>
   </si>
   <si>
     <t>agegroup_for_contact_tracing_pt</t>
@@ -820,10 +817,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D83"/>
+  <dimension ref="A1:D82"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="A47" sqref="A47"/>
+    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="A10" sqref="A10:XFD10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -932,7 +929,7 @@
         <v>0</v>
       </c>
       <c r="D8" s="14" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
@@ -950,23 +947,25 @@
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="10" t="s">
-        <v>52</v>
-      </c>
-      <c r="B10" s="10">
-        <v>0</v>
-      </c>
-      <c r="C10" s="10" t="s">
-        <v>0</v>
-      </c>
-      <c r="D10" s="10"/>
+      <c r="A10" s="8" t="s">
+        <v>99</v>
+      </c>
+      <c r="B10" s="8">
+        <v>200</v>
+      </c>
+      <c r="C10" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="D10" s="8" t="s">
+        <v>100</v>
+      </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="8" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="B11" s="8">
-        <v>200</v>
+        <v>20</v>
       </c>
       <c r="C11" s="8" t="s">
         <v>0</v>
@@ -977,30 +976,30 @@
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="8" t="s">
-        <v>99</v>
+        <v>20</v>
       </c>
       <c r="B12" s="8">
-        <v>20</v>
+        <v>100</v>
       </c>
       <c r="C12" s="8" t="s">
         <v>0</v>
       </c>
       <c r="D12" s="8" t="s">
-        <v>102</v>
+        <v>21</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="8" t="s">
-        <v>20</v>
+        <v>71</v>
       </c>
       <c r="B13" s="8">
-        <v>100</v>
+        <v>2</v>
       </c>
       <c r="C13" s="8" t="s">
         <v>0</v>
       </c>
       <c r="D13" s="8" t="s">
-        <v>21</v>
+        <v>73</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
@@ -1008,7 +1007,7 @@
         <v>72</v>
       </c>
       <c r="B14" s="8">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="C14" s="8" t="s">
         <v>0</v>
@@ -1017,66 +1016,66 @@
         <v>74</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" s="8" t="s">
-        <v>73</v>
-      </c>
-      <c r="B15" s="8">
-        <v>10</v>
-      </c>
-      <c r="C15" s="8" t="s">
-        <v>0</v>
-      </c>
-      <c r="D15" s="8" t="s">
+    <row r="15" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="13" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="16" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="13" t="s">
-        <v>76</v>
-      </c>
-      <c r="B16" s="13">
+      <c r="B15" s="13">
         <v>15.5</v>
       </c>
-      <c r="C16" s="13" t="s">
-        <v>0</v>
-      </c>
-      <c r="D16" s="13" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="11" t="s">
+      <c r="C15" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="D15" s="13" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="B17" s="11">
+      <c r="B16" s="11">
         <v>95</v>
       </c>
-      <c r="C17" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="D17" s="11" t="s">
+      <c r="C16" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="D16" s="11" t="s">
         <v>4</v>
       </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" s="6" t="s">
+        <v>110</v>
+      </c>
+      <c r="B17" s="6">
+        <v>0.7</v>
+      </c>
+      <c r="C17" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="D17" s="6"/>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="6" t="s">
         <v>111</v>
       </c>
       <c r="B18" s="6">
-        <v>0.7</v>
+        <v>15</v>
       </c>
       <c r="C18" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="D18" s="6"/>
+      <c r="D18" s="6" t="s">
+        <v>39</v>
+      </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="6" t="s">
         <v>112</v>
       </c>
       <c r="B19" s="6">
-        <v>15</v>
+        <v>30</v>
       </c>
       <c r="C19" s="6" t="s">
         <v>0</v>
@@ -1087,48 +1086,45 @@
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="6" t="s">
-        <v>113</v>
-      </c>
-      <c r="B20" s="6">
-        <v>30</v>
+        <v>11</v>
+      </c>
+      <c r="B20" s="6" t="b">
+        <v>1</v>
       </c>
       <c r="C20" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="D20" s="6" t="s">
-        <v>39</v>
-      </c>
+        <v>12</v>
+      </c>
+      <c r="D20" s="6"/>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="B21" s="6" t="b">
-        <v>1</v>
+        <v>13</v>
+      </c>
+      <c r="B21" s="6">
+        <v>3.0000000000000001E-3</v>
       </c>
       <c r="C21" s="6" t="s">
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="D21" s="6"/>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="6" t="s">
-        <v>13</v>
+        <v>109</v>
       </c>
       <c r="B22" s="6">
-        <v>3.0000000000000001E-3</v>
+        <v>0.75</v>
       </c>
       <c r="C22" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="D22" s="6"/>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="6" t="s">
-        <v>110</v>
+        <v>104</v>
       </c>
       <c r="B23" s="6">
-        <v>0.75</v>
+        <v>0.5</v>
       </c>
       <c r="C23" s="6" t="s">
         <v>0</v>
@@ -1139,7 +1135,7 @@
         <v>105</v>
       </c>
       <c r="B24" s="6">
-        <v>0.5</v>
+        <v>0.34</v>
       </c>
       <c r="C24" s="6" t="s">
         <v>0</v>
@@ -1150,7 +1146,7 @@
         <v>106</v>
       </c>
       <c r="B25" s="6">
-        <v>0.34</v>
+        <v>0.45</v>
       </c>
       <c r="C25" s="6" t="s">
         <v>0</v>
@@ -1161,60 +1157,61 @@
         <v>107</v>
       </c>
       <c r="B26" s="6">
-        <v>0.45</v>
+        <v>1</v>
       </c>
       <c r="C26" s="6" t="s">
         <v>0</v>
+      </c>
+      <c r="D26" t="s">
+        <v>108</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" s="6" t="s">
-        <v>108</v>
+        <v>28</v>
       </c>
       <c r="B27" s="6">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="C27" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="D27" t="s">
-        <v>109</v>
+      <c r="D27" s="14" t="s">
+        <v>103</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" s="6" t="s">
-        <v>28</v>
+        <v>102</v>
       </c>
       <c r="B28" s="6">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="C28" s="6" t="s">
         <v>0</v>
       </c>
       <c r="D28" s="14" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" s="6" t="s">
-        <v>103</v>
+        <v>29</v>
       </c>
       <c r="B29" s="6">
-        <v>15</v>
+        <v>0.5</v>
       </c>
       <c r="C29" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="D29" s="14" t="s">
-        <v>104</v>
-      </c>
+      <c r="D29" s="6"/>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" s="6" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B30" s="6">
-        <v>0.5</v>
+        <v>0.25</v>
       </c>
       <c r="C30" s="6" t="s">
         <v>0</v>
@@ -1222,34 +1219,36 @@
       <c r="D30" s="6"/>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A31" s="6" t="s">
-        <v>30</v>
-      </c>
-      <c r="B31" s="6">
-        <v>0.25</v>
-      </c>
-      <c r="C31" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="D31" s="6"/>
+      <c r="A31" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B31" s="2">
+        <v>20</v>
+      </c>
+      <c r="C31" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D31" s="2" t="s">
+        <v>65</v>
+      </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B32" s="2">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>66</v>
+        <v>4</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
-        <v>34</v>
+        <v>82</v>
       </c>
       <c r="B33" s="2">
         <v>0</v>
@@ -1262,25 +1261,23 @@
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A34" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="B34" s="2">
-        <v>0</v>
-      </c>
-      <c r="C34" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="D34" s="2" t="s">
-        <v>4</v>
-      </c>
+      <c r="A34" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="B34" s="15">
+        <v>1.9E-2</v>
+      </c>
+      <c r="C34" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="D34" s="9"/>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" s="9" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B35" s="15">
-        <v>1.9E-2</v>
+        <v>1.4E-2</v>
       </c>
       <c r="C35" s="9" t="s">
         <v>0</v>
@@ -1289,10 +1286,10 @@
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" s="9" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B36" s="15">
-        <v>1.4E-2</v>
+        <v>5.5999999999999999E-3</v>
       </c>
       <c r="C36" s="9" t="s">
         <v>0</v>
@@ -1301,10 +1298,10 @@
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" s="9" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B37" s="15">
-        <v>5.5999999999999999E-3</v>
+        <v>3.3999999999999999E-11</v>
       </c>
       <c r="C37" s="9" t="s">
         <v>0</v>
@@ -1313,10 +1310,10 @@
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" s="9" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B38" s="15">
-        <v>3.3999999999999999E-11</v>
+        <v>6.3999999999999997E-6</v>
       </c>
       <c r="C38" s="9" t="s">
         <v>0</v>
@@ -1325,10 +1322,10 @@
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" s="9" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B39" s="15">
-        <v>6.3999999999999997E-6</v>
+        <v>3.3000000000000002E-6</v>
       </c>
       <c r="C39" s="9" t="s">
         <v>0</v>
@@ -1337,28 +1334,30 @@
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="B40" s="15">
-        <v>3.3000000000000002E-6</v>
+        <v>92</v>
+      </c>
+      <c r="B40" s="9">
+        <v>0.65</v>
       </c>
       <c r="C40" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="D40" s="9"/>
+      <c r="D40" s="9" t="s">
+        <v>95</v>
+      </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" s="9" t="s">
         <v>93</v>
       </c>
       <c r="B41" s="9">
-        <v>0.65</v>
+        <v>0.81</v>
       </c>
       <c r="C41" s="9" t="s">
         <v>0</v>
       </c>
       <c r="D41" s="9" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
@@ -1366,73 +1365,73 @@
         <v>94</v>
       </c>
       <c r="B42" s="9">
-        <v>0.81</v>
+        <v>0.95</v>
       </c>
       <c r="C42" s="9" t="s">
         <v>0</v>
       </c>
       <c r="D42" s="9" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A43" s="9" t="s">
-        <v>95</v>
-      </c>
-      <c r="B43" s="9">
-        <v>0.95</v>
-      </c>
-      <c r="C43" s="9" t="s">
-        <v>0</v>
-      </c>
-      <c r="D43" s="9" t="s">
-        <v>96</v>
-      </c>
+      <c r="A43" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B43" s="1">
+        <v>50</v>
+      </c>
+      <c r="C43" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D43" s="1"/>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="B44" s="1">
+        <v>25</v>
+      </c>
+      <c r="C44" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D44" s="1"/>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A45" s="16" t="s">
+        <v>25</v>
+      </c>
+      <c r="B45" s="16">
         <v>27</v>
       </c>
-      <c r="B44" s="1">
-        <v>50</v>
-      </c>
-      <c r="C44" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D44" s="1"/>
-    </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A45" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="B45" s="1">
-        <v>25</v>
-      </c>
-      <c r="C45" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D45" s="1"/>
+      <c r="C45" s="16" t="s">
+        <v>0</v>
+      </c>
+      <c r="D45" s="16" t="s">
+        <v>116</v>
+      </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" s="16" t="s">
-        <v>25</v>
+        <v>68</v>
       </c>
       <c r="B46" s="16">
-        <v>27</v>
+        <v>52</v>
       </c>
       <c r="C46" s="16" t="s">
         <v>0</v>
       </c>
       <c r="D46" s="16" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" s="16" t="s">
-        <v>69</v>
+        <v>26</v>
       </c>
       <c r="B47" s="16">
-        <v>52</v>
+        <v>0.33600000000000002</v>
       </c>
       <c r="C47" s="16" t="s">
         <v>0</v>
@@ -1443,30 +1442,30 @@
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" s="16" t="s">
-        <v>26</v>
+        <v>69</v>
       </c>
       <c r="B48" s="16">
-        <v>0.33600000000000002</v>
+        <v>5.8000000000000003E-2</v>
       </c>
       <c r="C48" s="16" t="s">
         <v>0</v>
       </c>
       <c r="D48" s="16" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A49" s="5" t="s">
         <v>118</v>
       </c>
-    </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A49" s="16" t="s">
-        <v>70</v>
-      </c>
-      <c r="B49" s="16">
-        <v>5.8000000000000003E-2</v>
-      </c>
-      <c r="C49" s="16" t="s">
-        <v>0</v>
-      </c>
-      <c r="D49" s="16" t="s">
-        <v>118</v>
+      <c r="B49" s="5">
+        <v>0.23300000000000001</v>
+      </c>
+      <c r="C49" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="D49" s="5" t="s">
+        <v>121</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
@@ -1474,13 +1473,13 @@
         <v>119</v>
       </c>
       <c r="B50" s="5">
-        <v>0.23300000000000001</v>
+        <v>0.14699999999999999</v>
       </c>
       <c r="C50" s="5" t="s">
         <v>0</v>
       </c>
       <c r="D50" s="5" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
@@ -1488,119 +1487,119 @@
         <v>120</v>
       </c>
       <c r="B51" s="5">
-        <v>0.14699999999999999</v>
+        <v>0.39</v>
       </c>
       <c r="C51" s="5" t="s">
         <v>0</v>
       </c>
       <c r="D51" s="5" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52" s="5" t="s">
+        <v>122</v>
+      </c>
+      <c r="B52" s="5">
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="C52" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="D52" s="5" t="s">
         <v>121</v>
       </c>
-      <c r="B52" s="5">
-        <v>0.39</v>
-      </c>
-      <c r="C52" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="D52" s="5" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A53" s="5" t="s">
-        <v>123</v>
-      </c>
-      <c r="B53" s="5">
-        <v>2.5000000000000001E-2</v>
-      </c>
-      <c r="C53" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="D53" s="5" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="54" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A54" s="1" t="s">
-        <v>97</v>
-      </c>
-      <c r="B54" s="1">
+    </row>
+    <row r="53" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A53" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="B53" s="1">
         <v>0.21</v>
       </c>
-      <c r="C54" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D54" s="1"/>
-    </row>
-    <row r="55" spans="1:4" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A55" s="12" t="s">
+      <c r="C53" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D53" s="1"/>
+    </row>
+    <row r="54" spans="1:4" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A54" s="12" t="s">
         <v>31</v>
       </c>
-      <c r="B55" s="12">
+      <c r="B54" s="12">
         <v>77</v>
       </c>
-      <c r="C55" s="12" t="s">
-        <v>0</v>
-      </c>
-      <c r="D55" s="12"/>
+      <c r="C54" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="D54" s="12"/>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A55" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="B55" s="4">
+        <v>77</v>
+      </c>
+      <c r="C55" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="D55" s="4"/>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A56" s="4" t="s">
-        <v>71</v>
+        <v>23</v>
       </c>
       <c r="B56" s="4">
-        <v>77</v>
+        <v>7</v>
       </c>
       <c r="C56" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="D56" s="4"/>
+      <c r="D56" s="4" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A57" s="4" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B57" s="4">
-        <v>7</v>
+        <v>92</v>
       </c>
       <c r="C57" s="4" t="s">
         <v>0</v>
       </c>
       <c r="D57" s="4" t="s">
-        <v>22</v>
+        <v>64</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A58" s="4" t="s">
-        <v>24</v>
+        <v>83</v>
       </c>
       <c r="B58" s="4">
-        <v>92</v>
+        <v>0.6</v>
       </c>
       <c r="C58" s="4" t="s">
         <v>0</v>
       </c>
       <c r="D58" s="4" t="s">
-        <v>65</v>
+        <v>84</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A59" s="4" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="B59" s="4">
-        <v>0.6</v>
+        <v>50</v>
       </c>
       <c r="C59" s="4" t="s">
         <v>0</v>
       </c>
       <c r="D59" s="4" t="s">
-        <v>85</v>
+        <v>4</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.25">
@@ -1608,63 +1607,61 @@
         <v>86</v>
       </c>
       <c r="B60" s="4">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="C60" s="4" t="s">
         <v>0</v>
       </c>
       <c r="D60" s="4" t="s">
-        <v>4</v>
+        <v>87</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A61" s="4" t="s">
-        <v>87</v>
-      </c>
-      <c r="B61" s="4">
-        <v>0</v>
-      </c>
-      <c r="C61" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="D61" s="4" t="s">
-        <v>88</v>
+      <c r="A61" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="B61" s="7">
+        <v>0</v>
+      </c>
+      <c r="C61" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="D61" s="7" t="s">
+        <v>97</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A62" s="7" t="s">
-        <v>38</v>
-      </c>
-      <c r="B62" s="7">
-        <v>0</v>
-      </c>
-      <c r="C62" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="D62" s="7" t="s">
-        <v>98</v>
+      <c r="A62" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="B62" s="5">
+        <v>0.6</v>
+      </c>
+      <c r="C62" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="D62" s="5" t="s">
+        <v>66</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A63" s="5" t="s">
-        <v>32</v>
+        <v>41</v>
       </c>
       <c r="B63" s="5">
-        <v>0.6</v>
+        <v>0.84</v>
       </c>
       <c r="C63" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="D63" s="5" t="s">
-        <v>67</v>
-      </c>
+      <c r="D63" s="5"/>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A64" s="5" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
       <c r="B64" s="5">
-        <v>0.84</v>
+        <v>0.95</v>
       </c>
       <c r="C64" s="5" t="s">
         <v>0</v>
@@ -1673,10 +1670,10 @@
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A65" s="5" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="B65" s="5">
-        <v>0.95</v>
+        <v>0.8</v>
       </c>
       <c r="C65" s="5" t="s">
         <v>0</v>
@@ -1684,104 +1681,106 @@
       <c r="D65" s="5"/>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A66" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="B66" s="5">
-        <v>0.8</v>
-      </c>
-      <c r="C66" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="D66" s="5"/>
+      <c r="A66" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B66" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="C66" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D66" s="1"/>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A67" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="B67" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="C67" s="1" t="s">
+      <c r="A67" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="B67" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="C67" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="D67" s="1"/>
+      <c r="D67" s="3"/>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A68" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="B68" s="3" t="b">
-        <v>0</v>
+        <v>37</v>
+      </c>
+      <c r="B68" s="3">
+        <v>10</v>
       </c>
       <c r="C68" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="D68" s="3"/>
+        <v>0</v>
+      </c>
+      <c r="D68" s="3" t="s">
+        <v>40</v>
+      </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A69" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="B69" s="3">
-        <v>10</v>
+        <v>43</v>
+      </c>
+      <c r="B69" s="3" t="s">
+        <v>45</v>
       </c>
       <c r="C69" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="D69" s="3" t="s">
-        <v>40</v>
-      </c>
+        <v>44</v>
+      </c>
+      <c r="D69" s="3"/>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A70" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="B70" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="C70" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="D70" s="3"/>
+      <c r="A70" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="B70" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="C70" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="D70" s="6"/>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A71" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="B71" s="6" t="b">
-        <v>0</v>
+        <v>53</v>
+      </c>
+      <c r="B71" s="6" t="s">
+        <v>45</v>
       </c>
       <c r="C71" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="D71" s="6"/>
+        <v>44</v>
+      </c>
+      <c r="D71" s="6" t="s">
+        <v>54</v>
+      </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A72" s="6" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B72" s="6" t="s">
-        <v>45</v>
+        <v>58</v>
       </c>
       <c r="C72" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="D72" s="6" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D72" s="6"/>
+    </row>
+    <row r="73" spans="1:4" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A73" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="B73" s="6" t="s">
-        <v>59</v>
+        <v>78</v>
+      </c>
+      <c r="B73" s="6">
+        <v>0</v>
       </c>
       <c r="C73" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="D73" s="6"/>
+        <v>0</v>
+      </c>
+      <c r="D73" s="6" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="74" spans="1:4" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A74" s="6" t="s">
@@ -1797,7 +1796,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="75" spans="1:4" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A75" s="6" t="s">
         <v>80</v>
       </c>
@@ -1813,56 +1812,56 @@
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A76" s="6" t="s">
-        <v>81</v>
-      </c>
-      <c r="B76" s="6">
-        <v>0</v>
+        <v>60</v>
+      </c>
+      <c r="B76" s="6" t="s">
+        <v>45</v>
       </c>
       <c r="C76" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="D76" s="6" t="s">
-        <v>4</v>
-      </c>
+        <v>44</v>
+      </c>
+      <c r="D76" s="6"/>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A77" s="6" t="s">
         <v>61</v>
       </c>
-      <c r="B77" s="6" t="s">
-        <v>45</v>
+      <c r="B77" s="6">
+        <v>7</v>
       </c>
       <c r="C77" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="D77" s="6"/>
+        <v>0</v>
+      </c>
+      <c r="D77" s="6" t="s">
+        <v>62</v>
+      </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A78" s="6" t="s">
-        <v>62</v>
+        <v>88</v>
       </c>
       <c r="B78" s="6">
-        <v>7</v>
+        <v>100</v>
       </c>
       <c r="C78" s="6" t="s">
         <v>0</v>
       </c>
       <c r="D78" s="6" t="s">
-        <v>63</v>
+        <v>89</v>
       </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A79" s="6" t="s">
+        <v>90</v>
+      </c>
+      <c r="B79" s="6">
+        <v>50</v>
+      </c>
+      <c r="C79" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="D79" s="6" t="s">
         <v>89</v>
-      </c>
-      <c r="B79" s="6">
-        <v>100</v>
-      </c>
-      <c r="C79" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="D79" s="6" t="s">
-        <v>90</v>
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.25">
@@ -1870,51 +1869,37 @@
         <v>91</v>
       </c>
       <c r="B80" s="6">
-        <v>50</v>
+        <v>150</v>
       </c>
       <c r="C80" s="6" t="s">
         <v>0</v>
       </c>
       <c r="D80" s="6" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A81" s="6" t="s">
-        <v>92</v>
+        <v>113</v>
       </c>
       <c r="B81" s="6">
-        <v>150</v>
+        <v>15</v>
       </c>
       <c r="C81" s="6" t="s">
         <v>0</v>
       </c>
       <c r="D81" s="6" t="s">
-        <v>90</v>
+        <v>114</v>
       </c>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A82" s="6" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="B82" s="6">
-        <v>15</v>
+        <v>1</v>
       </c>
       <c r="C82" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="D82" s="6" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A83" s="6" t="s">
-        <v>116</v>
-      </c>
-      <c r="B83" s="6">
-        <v>1</v>
-      </c>
-      <c r="C83" s="6" t="s">
         <v>0</v>
       </c>
     </row>
@@ -1928,19 +1913,19 @@
           <x14:formula1>
             <xm:f>dropdown!$C$1:$C$3</xm:f>
           </x14:formula1>
-          <xm:sqref>B70 B73</xm:sqref>
+          <xm:sqref>B69 B72</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-000001000000}">
           <x14:formula1>
             <xm:f>dropdown!$A$1:$A$5</xm:f>
           </x14:formula1>
-          <xm:sqref>B72</xm:sqref>
+          <xm:sqref>B71</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-000002000000}">
           <x14:formula1>
             <xm:f>dropdown!$E$1:$E$5</xm:f>
           </x14:formula1>
-          <xm:sqref>B77</xm:sqref>
+          <xm:sqref>B76</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -1971,40 +1956,40 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E4" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="E5" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Remove old parameters for TB NH
</commit_message>
<xml_diff>
--- a/spreadsheets/common_parameters.xlsx
+++ b/spreadsheets/common_parameters.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rrag0004\Models\SNAP-TB\spreadsheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C28166B9-F30C-4BA2-BD6A-FECAAF51D2B5}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B68CFD8-25E0-45CF-A9C9-336E15F48F14}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="16395" windowHeight="6600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="228" uniqueCount="123">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="216" uniqueCount="117">
   <si>
     <t>float</t>
   </si>
@@ -103,12 +103,6 @@
     <t>perc_treatment_success</t>
   </si>
   <si>
-    <t>perc_sp_cure_smearpos</t>
-  </si>
-  <si>
-    <t>lambda_timeto_sp_or_death_smearpos</t>
-  </si>
-  <si>
     <t>perc_smearpos</t>
   </si>
   <si>
@@ -232,12 +226,6 @@
     <t>perc_extrapulmonary</t>
   </si>
   <si>
-    <t>perc_sp_cure_closed_tb</t>
-  </si>
-  <si>
-    <t>lambda_timeto_sp_or_death_closed_tb</t>
-  </si>
-  <si>
     <t>perc_cdr_closed_tb</t>
   </si>
   <si>
@@ -374,12 +362,6 @@
   </si>
   <si>
     <t>tb_mortality_multiplier</t>
-  </si>
-  <si>
-    <t>old tbnh params</t>
-  </si>
-  <si>
-    <t>!!! Unit Year-1     old tbnh params</t>
   </si>
   <si>
     <t>rate_sp_cure_smearpos</t>
@@ -493,7 +475,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="2" tint="-0.499984740745262"/>
+        <fgColor theme="3" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -817,10 +799,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D82"/>
+  <dimension ref="A1:D78"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10:XFD10"/>
+    <sheetView tabSelected="1" topLeftCell="A31" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
+      <selection activeCell="A49" sqref="A49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -832,7 +814,7 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="9" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B1" s="9">
         <v>1000</v>
@@ -858,7 +840,7 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="10" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B3" s="10">
         <v>18</v>
@@ -870,7 +852,7 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="10" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B4" s="10">
         <v>30</v>
@@ -882,7 +864,7 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="10" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B5" s="10">
         <v>10</v>
@@ -891,7 +873,7 @@
         <v>0</v>
       </c>
       <c r="D5" s="10" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -929,7 +911,7 @@
         <v>0</v>
       </c>
       <c r="D8" s="14" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
@@ -948,7 +930,7 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="8" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="B10" s="8">
         <v>200</v>
@@ -957,12 +939,12 @@
         <v>0</v>
       </c>
       <c r="D10" s="8" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="8" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="B11" s="8">
         <v>20</v>
@@ -971,7 +953,7 @@
         <v>0</v>
       </c>
       <c r="D11" s="8" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
@@ -990,7 +972,7 @@
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="8" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="B13" s="8">
         <v>2</v>
@@ -999,12 +981,12 @@
         <v>0</v>
       </c>
       <c r="D13" s="8" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="8" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="B14" s="8">
         <v>10</v>
@@ -1013,12 +995,12 @@
         <v>0</v>
       </c>
       <c r="D14" s="8" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="13" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="B15" s="13">
         <v>15.5</v>
@@ -1027,7 +1009,7 @@
         <v>0</v>
       </c>
       <c r="D15" s="13" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
@@ -1046,7 +1028,7 @@
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="6" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="B17" s="6">
         <v>0.7</v>
@@ -1058,7 +1040,7 @@
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="6" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="B18" s="6">
         <v>15</v>
@@ -1067,12 +1049,12 @@
         <v>0</v>
       </c>
       <c r="D18" s="6" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="6" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="B19" s="6">
         <v>30</v>
@@ -1081,7 +1063,7 @@
         <v>0</v>
       </c>
       <c r="D19" s="6" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
@@ -1110,7 +1092,7 @@
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="6" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="B22" s="6">
         <v>0.75</v>
@@ -1121,7 +1103,7 @@
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="6" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="B23" s="6">
         <v>0.5</v>
@@ -1132,7 +1114,7 @@
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="6" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="B24" s="6">
         <v>0.34</v>
@@ -1143,7 +1125,7 @@
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="6" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="B25" s="6">
         <v>0.45</v>
@@ -1154,7 +1136,7 @@
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="6" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="B26" s="6">
         <v>1</v>
@@ -1163,12 +1145,12 @@
         <v>0</v>
       </c>
       <c r="D26" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" s="6" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B27" s="6">
         <v>10</v>
@@ -1177,12 +1159,12 @@
         <v>0</v>
       </c>
       <c r="D27" s="14" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" s="6" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="B28" s="6">
         <v>15</v>
@@ -1191,12 +1173,12 @@
         <v>0</v>
       </c>
       <c r="D28" s="14" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" s="6" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B29" s="6">
         <v>0.5</v>
@@ -1208,7 +1190,7 @@
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" s="6" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B30" s="6">
         <v>0.25</v>
@@ -1220,7 +1202,7 @@
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B31" s="2">
         <v>20</v>
@@ -1229,12 +1211,12 @@
         <v>1</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B32" s="2">
         <v>0</v>
@@ -1248,7 +1230,7 @@
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="B33" s="2">
         <v>0</v>
@@ -1334,7 +1316,7 @@
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" s="9" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="B40" s="9">
         <v>0.65</v>
@@ -1343,12 +1325,12 @@
         <v>0</v>
       </c>
       <c r="D40" s="9" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" s="9" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="B41" s="9">
         <v>0.81</v>
@@ -1357,12 +1339,12 @@
         <v>0</v>
       </c>
       <c r="D41" s="9" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" s="9" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="B42" s="9">
         <v>0.95</v>
@@ -1371,12 +1353,12 @@
         <v>0</v>
       </c>
       <c r="D42" s="9" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B43" s="1">
         <v>50</v>
@@ -1388,7 +1370,7 @@
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="B44" s="1">
         <v>25</v>
@@ -1399,509 +1381,454 @@
       <c r="D44" s="1"/>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A45" s="16" t="s">
-        <v>25</v>
-      </c>
-      <c r="B45" s="16">
-        <v>27</v>
-      </c>
-      <c r="C45" s="16" t="s">
-        <v>0</v>
-      </c>
-      <c r="D45" s="16" t="s">
+      <c r="A45" s="5" t="s">
+        <v>112</v>
+      </c>
+      <c r="B45" s="5">
+        <v>0.23300000000000001</v>
+      </c>
+      <c r="C45" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="D45" s="5" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A46" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="B46" s="5">
+        <v>0.14699999999999999</v>
+      </c>
+      <c r="C46" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="D46" s="5" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A47" s="5" t="s">
+        <v>114</v>
+      </c>
+      <c r="B47" s="5">
+        <v>0.39</v>
+      </c>
+      <c r="C47" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="D47" s="5" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A48" s="5" t="s">
         <v>116</v>
       </c>
-    </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A46" s="16" t="s">
-        <v>68</v>
-      </c>
-      <c r="B46" s="16">
-        <v>52</v>
-      </c>
-      <c r="C46" s="16" t="s">
-        <v>0</v>
-      </c>
-      <c r="D46" s="16" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A47" s="16" t="s">
-        <v>26</v>
-      </c>
-      <c r="B47" s="16">
-        <v>0.33600000000000002</v>
-      </c>
-      <c r="C47" s="16" t="s">
-        <v>0</v>
-      </c>
-      <c r="D47" s="16" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A48" s="16" t="s">
-        <v>69</v>
-      </c>
-      <c r="B48" s="16">
-        <v>5.8000000000000003E-2</v>
-      </c>
-      <c r="C48" s="16" t="s">
-        <v>0</v>
-      </c>
-      <c r="D48" s="16" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A49" s="5" t="s">
-        <v>118</v>
-      </c>
-      <c r="B49" s="5">
-        <v>0.23300000000000001</v>
-      </c>
-      <c r="C49" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="D49" s="5" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A50" s="5" t="s">
-        <v>119</v>
-      </c>
-      <c r="B50" s="5">
-        <v>0.14699999999999999</v>
-      </c>
-      <c r="C50" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="D50" s="5" t="s">
-        <v>121</v>
-      </c>
+      <c r="B48" s="5">
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="C48" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="D48" s="5" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A49" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="B49" s="1">
+        <v>0.21</v>
+      </c>
+      <c r="C49" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D49" s="1"/>
+    </row>
+    <row r="50" spans="1:4" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A50" s="12" t="s">
+        <v>29</v>
+      </c>
+      <c r="B50" s="12">
+        <v>77</v>
+      </c>
+      <c r="C50" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="D50" s="12"/>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A51" s="5" t="s">
-        <v>120</v>
-      </c>
-      <c r="B51" s="5">
-        <v>0.39</v>
-      </c>
-      <c r="C51" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="D51" s="5" t="s">
-        <v>121</v>
-      </c>
+      <c r="A51" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="B51" s="4">
+        <v>77</v>
+      </c>
+      <c r="C51" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="D51" s="4"/>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A52" s="5" t="s">
-        <v>122</v>
-      </c>
-      <c r="B52" s="5">
-        <v>2.5000000000000001E-2</v>
-      </c>
-      <c r="C52" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="D52" s="5" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="53" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A53" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="B53" s="1">
-        <v>0.21</v>
-      </c>
-      <c r="C53" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D53" s="1"/>
-    </row>
-    <row r="54" spans="1:4" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A54" s="12" t="s">
-        <v>31</v>
-      </c>
-      <c r="B54" s="12">
-        <v>77</v>
-      </c>
-      <c r="C54" s="12" t="s">
-        <v>0</v>
-      </c>
-      <c r="D54" s="12"/>
+      <c r="A52" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="B52" s="4">
+        <v>7</v>
+      </c>
+      <c r="C52" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="D52" s="4" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A53" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="B53" s="4">
+        <v>92</v>
+      </c>
+      <c r="C53" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="D53" s="4" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A54" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="B54" s="4">
+        <v>0.6</v>
+      </c>
+      <c r="C54" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="D54" s="4" t="s">
+        <v>80</v>
+      </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A55" s="4" t="s">
-        <v>70</v>
+        <v>81</v>
       </c>
       <c r="B55" s="4">
-        <v>77</v>
+        <v>50</v>
       </c>
       <c r="C55" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="D55" s="4"/>
+      <c r="D55" s="4" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A56" s="4" t="s">
-        <v>23</v>
+        <v>82</v>
       </c>
       <c r="B56" s="4">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="C56" s="4" t="s">
         <v>0</v>
       </c>
       <c r="D56" s="4" t="s">
-        <v>22</v>
+        <v>83</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A57" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="B57" s="4">
-        <v>92</v>
-      </c>
-      <c r="C57" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="D57" s="4" t="s">
+      <c r="A57" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="B57" s="7">
+        <v>0</v>
+      </c>
+      <c r="C57" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="D57" s="7" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A58" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="B58" s="5">
+        <v>0.6</v>
+      </c>
+      <c r="C58" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="D58" s="5" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A58" s="4" t="s">
-        <v>83</v>
-      </c>
-      <c r="B58" s="4">
-        <v>0.6</v>
-      </c>
-      <c r="C58" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="D58" s="4" t="s">
-        <v>84</v>
-      </c>
-    </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A59" s="4" t="s">
-        <v>85</v>
-      </c>
-      <c r="B59" s="4">
+      <c r="A59" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="B59" s="5">
+        <v>0.84</v>
+      </c>
+      <c r="C59" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="D59" s="5"/>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A60" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="B60" s="5">
+        <v>0.95</v>
+      </c>
+      <c r="C60" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="D60" s="5"/>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A61" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="B61" s="5">
+        <v>0.8</v>
+      </c>
+      <c r="C61" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="D61" s="5"/>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A62" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="B62" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="C62" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D62" s="1"/>
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A63" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="B63" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="C63" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D63" s="3"/>
+    </row>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A64" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="B64" s="3">
+        <v>10</v>
+      </c>
+      <c r="C64" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="D64" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A65" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="B65" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="C65" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="D65" s="3"/>
+    </row>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A66" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="B66" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="C66" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="D66" s="6"/>
+    </row>
+    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A67" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="B67" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="C67" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="D67" s="6" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A68" s="6" t="s">
         <v>50</v>
       </c>
-      <c r="C59" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="D59" s="4" t="s">
+      <c r="B68" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="C68" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="D68" s="6"/>
+    </row>
+    <row r="69" spans="1:4" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A69" s="6" t="s">
+        <v>74</v>
+      </c>
+      <c r="B69" s="6">
+        <v>0</v>
+      </c>
+      <c r="C69" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="D69" s="6" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A60" s="4" t="s">
-        <v>86</v>
-      </c>
-      <c r="B60" s="4">
-        <v>0</v>
-      </c>
-      <c r="C60" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="D60" s="4" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A61" s="7" t="s">
-        <v>38</v>
-      </c>
-      <c r="B61" s="7">
-        <v>0</v>
-      </c>
-      <c r="C61" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="D61" s="7" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A62" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="B62" s="5">
-        <v>0.6</v>
-      </c>
-      <c r="C62" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="D62" s="5" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A63" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="B63" s="5">
-        <v>0.84</v>
-      </c>
-      <c r="C63" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="D63" s="5"/>
-    </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A64" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="B64" s="5">
-        <v>0.95</v>
-      </c>
-      <c r="C64" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="D64" s="5"/>
-    </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A65" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="B65" s="5">
-        <v>0.8</v>
-      </c>
-      <c r="C65" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="D65" s="5"/>
-    </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A66" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="B66" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="C66" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="D66" s="1"/>
-    </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A67" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="B67" s="3" t="b">
-        <v>0</v>
-      </c>
-      <c r="C67" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="D67" s="3"/>
-    </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A68" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="B68" s="3">
-        <v>10</v>
-      </c>
-      <c r="C68" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="D68" s="3" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A69" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="B69" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="C69" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="D69" s="3"/>
-    </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:4" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A70" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="B70" s="6" t="b">
+        <v>75</v>
+      </c>
+      <c r="B70" s="6">
         <v>0</v>
       </c>
       <c r="C70" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="D70" s="6"/>
+        <v>0</v>
+      </c>
+      <c r="D70" s="6" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A71" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="B71" s="6" t="s">
-        <v>45</v>
+        <v>76</v>
+      </c>
+      <c r="B71" s="6">
+        <v>0</v>
       </c>
       <c r="C71" s="6" t="s">
-        <v>44</v>
+        <v>0</v>
       </c>
       <c r="D71" s="6" t="s">
-        <v>54</v>
+        <v>4</v>
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A72" s="6" t="s">
-        <v>52</v>
+        <v>58</v>
       </c>
       <c r="B72" s="6" t="s">
-        <v>58</v>
+        <v>43</v>
       </c>
       <c r="C72" s="6" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="D72" s="6"/>
     </row>
-    <row r="73" spans="1:4" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A73" s="6" t="s">
-        <v>78</v>
+        <v>59</v>
       </c>
       <c r="B73" s="6">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="C73" s="6" t="s">
         <v>0</v>
       </c>
       <c r="D73" s="6" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="74" spans="1:4" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A74" s="6" t="s">
-        <v>79</v>
-      </c>
-      <c r="B74" s="6">
-        <v>0</v>
-      </c>
-      <c r="C74" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="D74" s="6" t="s">
-        <v>4</v>
+        <v>60</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A74" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="B74" s="1">
+        <v>100</v>
+      </c>
+      <c r="C74" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D74" s="1" t="s">
+        <v>85</v>
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A75" s="6" t="s">
-        <v>80</v>
-      </c>
-      <c r="B75" s="6">
-        <v>0</v>
-      </c>
-      <c r="C75" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="D75" s="6" t="s">
-        <v>4</v>
+      <c r="A75" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="B75" s="1">
+        <v>50</v>
+      </c>
+      <c r="C75" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D75" s="1" t="s">
+        <v>85</v>
       </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A76" s="6" t="s">
-        <v>60</v>
-      </c>
-      <c r="B76" s="6" t="s">
-        <v>45</v>
-      </c>
-      <c r="C76" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="D76" s="6"/>
+      <c r="A76" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="B76" s="1">
+        <v>150</v>
+      </c>
+      <c r="C76" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D76" s="1" t="s">
+        <v>85</v>
+      </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A77" s="6" t="s">
-        <v>61</v>
-      </c>
-      <c r="B77" s="6">
-        <v>7</v>
-      </c>
-      <c r="C77" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="D77" s="6" t="s">
-        <v>62</v>
+      <c r="A77" s="16" t="s">
+        <v>109</v>
+      </c>
+      <c r="B77" s="16">
+        <v>15</v>
+      </c>
+      <c r="C77" s="16" t="s">
+        <v>0</v>
+      </c>
+      <c r="D77" s="16" t="s">
+        <v>110</v>
       </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A78" s="6" t="s">
-        <v>88</v>
-      </c>
-      <c r="B78" s="6">
-        <v>100</v>
-      </c>
-      <c r="C78" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="D78" s="6" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A79" s="6" t="s">
-        <v>90</v>
-      </c>
-      <c r="B79" s="6">
-        <v>50</v>
-      </c>
-      <c r="C79" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="D79" s="6" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A80" s="6" t="s">
-        <v>91</v>
-      </c>
-      <c r="B80" s="6">
-        <v>150</v>
-      </c>
-      <c r="C80" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="D80" s="6" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A81" s="6" t="s">
-        <v>113</v>
-      </c>
-      <c r="B81" s="6">
-        <v>15</v>
-      </c>
-      <c r="C81" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="D81" s="6" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A82" s="6" t="s">
-        <v>115</v>
-      </c>
-      <c r="B82" s="6">
+      <c r="A78" s="16" t="s">
+        <v>111</v>
+      </c>
+      <c r="B78" s="16">
         <v>1</v>
       </c>
-      <c r="C82" s="6" t="s">
-        <v>0</v>
-      </c>
+      <c r="C78" s="16" t="s">
+        <v>0</v>
+      </c>
+      <c r="D78" s="16"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1913,19 +1840,19 @@
           <x14:formula1>
             <xm:f>dropdown!$C$1:$C$3</xm:f>
           </x14:formula1>
-          <xm:sqref>B69 B72</xm:sqref>
+          <xm:sqref>B65 B68</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-000001000000}">
           <x14:formula1>
             <xm:f>dropdown!$A$1:$A$5</xm:f>
           </x14:formula1>
-          <xm:sqref>B71</xm:sqref>
+          <xm:sqref>B67</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-000002000000}">
           <x14:formula1>
             <xm:f>dropdown!$E$1:$E$5</xm:f>
           </x14:formula1>
-          <xm:sqref>B76</xm:sqref>
+          <xm:sqref>B72</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -1945,51 +1872,51 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C1" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="E1" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>53</v>
+      </c>
+      <c r="C2" t="s">
         <v>55</v>
       </c>
-      <c r="C2" t="s">
-        <v>57</v>
-      </c>
       <c r="E2" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>54</v>
+      </c>
+      <c r="C3" t="s">
         <v>56</v>
       </c>
-      <c r="C3" t="s">
-        <v>58</v>
-      </c>
       <c r="E3" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="E4" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="E5" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
   </sheetData>

</xml_diff>